<commit_message>
statistics for feature deltas until 2017-09-14
</commit_message>
<xml_diff>
--- a/statistics/development_time.xlsx
+++ b/statistics/development_time.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\repositories\ProjectSPLDevelopment\statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\SPLTeamprojektMigrated\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F739897C-5A58-4C6C-9114-85B125019E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1305A4B8-27D9-4842-BC49-82AC33D04590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="37245" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={5F5C7311-F9E7-44ED-9D9B-C15344CDCD93}</author>
+    <author>tc={AC72BACD-71EF-416D-9911-3382A131988C}</author>
     <author>tc={EC9143AF-697E-4544-ABFB-F004AC1C52AD}</author>
   </authors>
   <commentList>
@@ -48,7 +49,15 @@
     (YYYY-MM-DDThh:mm)</t>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" shapeId="0" xr:uid="{EC9143AF-697E-4544-ABFB-F004AC1C52AD}">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{AC72BACD-71EF-416D-9911-3382A131988C}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    including fixes</t>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="2" shapeId="0" xr:uid="{EC9143AF-697E-4544-ABFB-F004AC1C52AD}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -61,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="90">
   <si>
     <t>Feature Name</t>
   </si>
@@ -271,13 +280,73 @@
   </si>
   <si>
     <t>56f7edfbba627a0f3b70004b5b024d4c5751f59c , be7b7ddc3187704df54a1881e968bc54c67a5f18</t>
+  </si>
+  <si>
+    <t>--- no directly mapped feature. Feature interaction ---</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Time.deltaj</t>
+  </si>
+  <si>
+    <t>2017-09-12T12:00</t>
+  </si>
+  <si>
+    <t>159185f640c85bc713e1c48995507f5a0793000f , ada993b7ec190866bcdad3b473e851c4e59e12a7 , b63ac462523cf58d33ea9df56905103b0788d689</t>
+  </si>
+  <si>
+    <t>TimeInfo.deltaj</t>
+  </si>
+  <si>
+    <t>be7b7ddc3187704df54a1881e968bc54c67a5f18</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>History.deltaj</t>
+  </si>
+  <si>
+    <t>2017-09-14T12:56</t>
+  </si>
+  <si>
+    <t>028b24d4123d99a63440d90e047072ea8b78c163 , fcd9433d99741ed26a5f711e9c20ed83201a0fec , 7110e08d8cb741128e9171ecd0e5f3f0e87565af , 689cab6a2f5d322dc2b77756be9e5473d25ce40b , 4ad07e920b07e988b2f658d3d83d915d6359dccc , 1b3431af08f8bef9c95e460bb82b1457e593717f , 604b55d2950474913e42d13dd429b000fb59538c , f1bc693f40e4f8ce9df1e817466ed0e8ac03c01d , 6736380c2240161c4cd15cef149185c198abba5a , e291f2960b28cee337f96d218202d83933e95a9b , fd6368d3e4f8e5ac0e6ae0536c95ae639f657573 , 39635450ad96fab166902468fa6f87a63d6ec6fe</t>
+  </si>
+  <si>
+    <t>bddbeeab8d7ef88c2f259e7cf94c5aad7812295e , 44af0cad1b3ef9adebc5a810f70fe5b47fa36cca , 39635450ad96fab166902468fa6f87a63d6ec6fe</t>
+  </si>
+  <si>
+    <t>Speedlimit</t>
+  </si>
+  <si>
+    <t>Speedlimit.deltaj</t>
+  </si>
+  <si>
+    <t>07e848285abf5e59825c32aa9ce400bb442d3b9e , 9c122a89147f0c9ba8d399c3bff95fbb847327b1 , 0a226f5b67c816bfff80caa73415d4811683f3b3 , be7eb36a59667d27db08f5bbf98a0ec208e3178d , c0c4bfee81b2f6f70616484f0130fdd81aa029de , a47486b9fc05cda39b93ed265e72182dd9d288bd</t>
+  </si>
+  <si>
+    <t>f2f9fa053d672612c05e4ce0ce05871be2474d2a</t>
+  </si>
+  <si>
+    <t>Carpooling</t>
+  </si>
+  <si>
+    <t>CarPool.deltaj</t>
+  </si>
+  <si>
+    <t>e457be4b9a0d075e75c408dcf671efe1f19fbd91 , dc8ce88adc9cd052df42ef35a49c58f23f55b6c9 , 4535ea97d1ea5bd077dc2dbedc2d3e5622a35b4b , 55e3e3d4194caf98cbbdd78a02bf623332825c07</t>
+  </si>
+  <si>
+    <t>24b00f1fff1f1d5681a19e644e77d1ede9ba0878 , 90c5f659a5bb8d81c0f9c2dcd86ee4cd31b4f638</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,12 +359,6 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -356,6 +419,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Michael Nieke" id="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" userId="Michael Nieke" providerId="None"/>
   <person displayName="Michael Nieke" id="{D79E35A8-37B6-4A3D-A377-51485C625214}" userId="4b7b0d639a377549" providerId="Windows Live"/>
 </personList>
 </file>
@@ -626,6 +690,9 @@
   <threadedComment ref="C1" dT="2021-06-23T13:16:16.31" personId="{D79E35A8-37B6-4A3D-A377-51485C625214}" id="{5F5C7311-F9E7-44ED-9D9B-C15344CDCD93}">
     <text>(YYYY-MM-DDThh:mm)</text>
   </threadedComment>
+  <threadedComment ref="E1" dT="2021-06-24T10:41:01.57" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{AC72BACD-71EF-416D-9911-3382A131988C}">
+    <text>including fixes</text>
+  </threadedComment>
   <threadedComment ref="O1" dT="2021-06-23T12:59:04.88" personId="{D79E35A8-37B6-4A3D-A377-51485C625214}" id="{EC9143AF-697E-4544-ABFB-F004AC1C52AD}">
     <text>not considered the last commit for migration to the new DeltaJ version</text>
   </threadedComment>
@@ -637,31 +704,32 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q11" sqref="Q11"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.81640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="25.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="55" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.28515625" style="8" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.26953125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -714,7 +782,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -767,7 +835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -820,7 +888,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -848,6 +916,9 @@
       <c r="I4" s="4">
         <v>10</v>
       </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
       <c r="L4" s="8" t="s">
         <v>57</v>
       </c>
@@ -867,7 +938,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="B5" t="s">
         <v>64</v>
       </c>
@@ -887,6 +961,9 @@
         <v>1</v>
       </c>
       <c r="I5" s="4"/>
+      <c r="K5">
+        <v>0</v>
+      </c>
       <c r="L5" s="8" t="s">
         <v>46</v>
       </c>
@@ -906,7 +983,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -959,7 +1036,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
@@ -981,6 +1058,9 @@
       <c r="H7" s="3">
         <v>1</v>
       </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
       <c r="L7" s="9" t="s">
         <v>52</v>
       </c>
@@ -1000,7 +1080,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>36</v>
       </c>
@@ -1028,6 +1108,9 @@
       <c r="I8" s="3">
         <v>8</v>
       </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
       <c r="L8" s="9" t="s">
         <v>46</v>
       </c>
@@ -1047,7 +1130,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -1075,6 +1158,9 @@
       <c r="I9" s="3">
         <v>5</v>
       </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
       <c r="L9" s="9" t="s">
         <v>50</v>
       </c>
@@ -1094,7 +1180,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
@@ -1147,7 +1233,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="B11" t="s">
         <v>44</v>
       </c>
@@ -1172,6 +1261,9 @@
       <c r="K11">
         <v>2</v>
       </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
       <c r="N11" s="1" t="s">
         <v>68</v>
       </c>
@@ -1185,7 +1277,257 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3">
+        <v>5</v>
+      </c>
+      <c r="I12" s="3">
+        <v>7</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="P12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="3">
+        <v>12</v>
+      </c>
+      <c r="H14" s="3">
+        <v>7</v>
+      </c>
+      <c r="I14" s="3">
+        <v>8</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O14">
+        <v>16</v>
+      </c>
+      <c r="P14" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="3">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3">
+        <v>9</v>
+      </c>
+      <c r="I15" s="3">
+        <v>13</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15">
+        <v>7</v>
+      </c>
+      <c r="P15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="3">
+        <v>4</v>
+      </c>
+      <c r="H16" s="3">
+        <v>4</v>
+      </c>
+      <c r="I16" s="3">
+        <v>8</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="M16" s="3">
+        <v>2</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16">
+        <v>6</v>
+      </c>
+      <c r="P16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
statistics until Sept 19
</commit_message>
<xml_diff>
--- a/statistics/development_time.xlsx
+++ b/statistics/development_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\SPLTeamprojektMigrated\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD6D180-72AA-46DE-B26E-00CE1BBF5F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C4F31-73A6-4F16-BBA9-C7A0FDB9E9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,6 +40,10 @@
     <author>tc={AC72BACD-71EF-416D-9911-3382A131988C}</author>
     <author>tc={9D598DD2-472C-4405-A9E5-98D424598411}</author>
     <author>tc={EC9143AF-697E-4544-ABFB-F004AC1C52AD}</author>
+    <author>tc={02B7A502-EA60-48C2-A4ED-6D65727931AC}</author>
+    <author>tc={6207ED8D-94FE-4AAF-8444-4D21B004E5BF}</author>
+    <author>tc={083D291C-1366-47CF-A1C9-0188B7497467}</author>
+    <author>tc={0850F9F9-4BB2-4AA3-B45A-D7482D0EB600}</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{5F5C7311-F9E7-44ED-9D9B-C15344CDCD93}">
@@ -74,12 +78,44 @@
     not considered the last commit for migration to the new DeltaJ version</t>
       </text>
     </comment>
+    <comment ref="D34" authorId="4" shapeId="0" xr:uid="{02B7A502-EA60-48C2-A4ED-6D65727931AC}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    before the feature was introduced</t>
+      </text>
+    </comment>
+    <comment ref="D37" authorId="5" shapeId="0" xr:uid="{6207ED8D-94FE-4AAF-8444-4D21B004E5BF}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    before feature was introduced</t>
+      </text>
+    </comment>
+    <comment ref="D38" authorId="6" shapeId="0" xr:uid="{083D291C-1366-47CF-A1C9-0188B7497467}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    before feature was introduced</t>
+      </text>
+    </comment>
+    <comment ref="D39" authorId="7" shapeId="0" xr:uid="{0850F9F9-4BB2-4AA3-B45A-D7482D0EB600}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    before feature was introduced</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="157">
   <si>
     <t>Feature Name</t>
   </si>
@@ -475,6 +511,81 @@
   </si>
   <si>
     <t>ada993b7ec190866bcdad3b473e851c4e59e12a7</t>
+  </si>
+  <si>
+    <t>2017-09-19T00:00</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>Wikipedia.deltaj</t>
+  </si>
+  <si>
+    <t>2017-09-19</t>
+  </si>
+  <si>
+    <t>088e63c17fd0919a2a437854cb164b946ae043fb</t>
+  </si>
+  <si>
+    <t>90c5f659a5bb8d81c0f9c2dcd86ee4cd31b4f638 , be7b7ddc3187704df54a1881e968bc54c67a5f18</t>
+  </si>
+  <si>
+    <t>2017-09-19T13:00</t>
+  </si>
+  <si>
+    <t>StandardZoom</t>
+  </si>
+  <si>
+    <t>Pedestrian</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>RouteHistory</t>
+  </si>
+  <si>
+    <t>BusStops</t>
+  </si>
+  <si>
+    <t>Taxi</t>
+  </si>
+  <si>
+    <t>GreaterZoom.deltaj</t>
+  </si>
+  <si>
+    <t>PedestrianRoute.deltaj</t>
+  </si>
+  <si>
+    <t>--- does not have a mapped delta. Is the standard functionality of routing. Just a marker feature ---</t>
+  </si>
+  <si>
+    <t>HistoryRouting.deltaj</t>
+  </si>
+  <si>
+    <t>BusStopsNearby.deltaj</t>
+  </si>
+  <si>
+    <t>Taxi.deltaj</t>
+  </si>
+  <si>
+    <t>265acb5d951dbbf88a6d44e344a7f3afef6b620d</t>
+  </si>
+  <si>
+    <t>79481348413dc28db428a14a80ae6f64bc42fd31 , 90c5f659a5bb8d81c0f9c2dcd86ee4cd31b4f638</t>
+  </si>
+  <si>
+    <t>9cfa39ac77e788a83de5b9aa09887cb1fb482459</t>
+  </si>
+  <si>
+    <t>7110e08d8cb741128e9171ecd0e5f3f0e87565af , 4ad07e920b07e988b2f658d3d83d915d6359dccc , 1b3431af08f8bef9c95e460bb82b1457e593717f , bddbeeab8d7ef88c2f259e7cf94c5aad7812295e , 44af0cad1b3ef9adebc5a810f70fe5b47fa36cca , e291f2960b28cee337f96d218202d83933e95a9b , fd6368d3e4f8e5ac0e6ae0536c95ae639f657573 , 39635450ad96fab166902468fa6f87a63d6ec6fe</t>
+  </si>
+  <si>
+    <t>265acb5d951dbbf88a6d44e344a7f3afef6b620d , 79481348413dc28db428a14a80ae6f64bc42fd31 , c04fbdb4f1f2a60ec02868c2ace2966d335c228b</t>
+  </si>
+  <si>
+    <t>9a5dd57dd84ced514d11626a14a2cc068ff4dfce</t>
   </si>
 </sst>
 </file>
@@ -496,12 +607,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -516,7 +633,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -535,6 +652,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -834,6 +953,18 @@
   <threadedComment ref="O1" dT="2021-06-23T12:59:04.88" personId="{D79E35A8-37B6-4A3D-A377-51485C625214}" id="{EC9143AF-697E-4544-ABFB-F004AC1C52AD}">
     <text>not considered the last commit for migration to the new DeltaJ version</text>
   </threadedComment>
+  <threadedComment ref="D34" dT="2021-06-25T12:05:07.49" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{02B7A502-EA60-48C2-A4ED-6D65727931AC}">
+    <text>before the feature was introduced</text>
+  </threadedComment>
+  <threadedComment ref="D37" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{6207ED8D-94FE-4AAF-8444-4D21B004E5BF}">
+    <text>before feature was introduced</text>
+  </threadedComment>
+  <threadedComment ref="D38" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{083D291C-1366-47CF-A1C9-0188B7497467}">
+    <text>before feature was introduced</text>
+  </threadedComment>
+  <threadedComment ref="D39" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{0850F9F9-4BB2-4AA3-B45A-D7482D0EB600}">
+    <text>before feature was introduced</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -842,8 +973,8 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P33" sqref="P33"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2416,6 +2547,311 @@
         <v>26</v>
       </c>
     </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G33" s="3">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+      <c r="K33" s="3">
+        <v>0</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="M33" s="3">
+        <v>2</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O33">
+        <v>2</v>
+      </c>
+      <c r="P33" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
+        <v>0</v>
+      </c>
+      <c r="L34" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="M34" s="3">
+        <v>2</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34">
+        <v>3</v>
+      </c>
+      <c r="P34" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0</v>
+      </c>
+      <c r="M35" s="3">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G37" s="3">
+        <v>8</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>3</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0</v>
+      </c>
+      <c r="M37" s="3">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O37">
+        <v>8</v>
+      </c>
+      <c r="P37" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="G38" s="3">
+        <v>3</v>
+      </c>
+      <c r="H38" s="3">
+        <v>5</v>
+      </c>
+      <c r="I38" s="3">
+        <v>4</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M38" s="3">
+        <v>1</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38">
+        <v>4</v>
+      </c>
+      <c r="P38" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" t="s">
+        <v>138</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <v>4</v>
+      </c>
+      <c r="I39" s="3">
+        <v>3</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M39" s="3">
+        <v>1</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39">
+        <v>2</v>
+      </c>
+      <c r="P39" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
all delta commit statistics extracted
</commit_message>
<xml_diff>
--- a/statistics/development_time.xlsx
+++ b/statistics/development_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\SPLTeamprojektMigrated\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C4F31-73A6-4F16-BBA9-C7A0FDB9E9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8AA33B-8183-459A-96D4-FC2AA22CD46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,6 +44,7 @@
     <author>tc={6207ED8D-94FE-4AAF-8444-4D21B004E5BF}</author>
     <author>tc={083D291C-1366-47CF-A1C9-0188B7497467}</author>
     <author>tc={0850F9F9-4BB2-4AA3-B45A-D7482D0EB600}</author>
+    <author>tc={E1EEB336-76F9-4E42-854F-F43347D1E75F}</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{5F5C7311-F9E7-44ED-9D9B-C15344CDCD93}">
@@ -78,7 +79,7 @@
     not considered the last commit for migration to the new DeltaJ version</t>
       </text>
     </comment>
-    <comment ref="D34" authorId="4" shapeId="0" xr:uid="{02B7A502-EA60-48C2-A4ED-6D65727931AC}">
+    <comment ref="D33" authorId="4" shapeId="0" xr:uid="{02B7A502-EA60-48C2-A4ED-6D65727931AC}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -86,7 +87,7 @@
     before the feature was introduced</t>
       </text>
     </comment>
-    <comment ref="D37" authorId="5" shapeId="0" xr:uid="{6207ED8D-94FE-4AAF-8444-4D21B004E5BF}">
+    <comment ref="D36" authorId="5" shapeId="0" xr:uid="{6207ED8D-94FE-4AAF-8444-4D21B004E5BF}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -94,7 +95,7 @@
     before feature was introduced</t>
       </text>
     </comment>
-    <comment ref="D38" authorId="6" shapeId="0" xr:uid="{083D291C-1366-47CF-A1C9-0188B7497467}">
+    <comment ref="D37" authorId="6" shapeId="0" xr:uid="{083D291C-1366-47CF-A1C9-0188B7497467}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -102,7 +103,15 @@
     before feature was introduced</t>
       </text>
     </comment>
-    <comment ref="D39" authorId="7" shapeId="0" xr:uid="{0850F9F9-4BB2-4AA3-B45A-D7482D0EB600}">
+    <comment ref="D38" authorId="7" shapeId="0" xr:uid="{0850F9F9-4BB2-4AA3-B45A-D7482D0EB600}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    before feature was introduced</t>
+      </text>
+    </comment>
+    <comment ref="D40" authorId="8" shapeId="0" xr:uid="{E1EEB336-76F9-4E42-854F-F43347D1E75F}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -115,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="190">
   <si>
     <t>Feature Name</t>
   </si>
@@ -222,9 +231,6 @@
     <t>Information.deltaj</t>
   </si>
   <si>
-    <t>--- no directly mapped feature. Code reuse ---</t>
-  </si>
-  <si>
     <t>LocationImages</t>
   </si>
   <si>
@@ -586,6 +592,108 @@
   </si>
   <si>
     <t>9a5dd57dd84ced514d11626a14a2cc068ff4dfce</t>
+  </si>
+  <si>
+    <t>Truck</t>
+  </si>
+  <si>
+    <t>FavoriteRoute</t>
+  </si>
+  <si>
+    <t>2017-09-20T00:00</t>
+  </si>
+  <si>
+    <t>--- does not have a mapped delta. Seems to be forgotten to be implemented? ---</t>
+  </si>
+  <si>
+    <t>FavoriteRoute.deltaj</t>
+  </si>
+  <si>
+    <t>4469fb6806856abaf60855817d533b2e9ccd0456</t>
+  </si>
+  <si>
+    <t>ArrivalTime</t>
+  </si>
+  <si>
+    <t>DepartureTime</t>
+  </si>
+  <si>
+    <t>SuggestionFav</t>
+  </si>
+  <si>
+    <t>SuggestionHistory</t>
+  </si>
+  <si>
+    <t>InfoGroup</t>
+  </si>
+  <si>
+    <t>TextToSpeech</t>
+  </si>
+  <si>
+    <t>TTSNavi</t>
+  </si>
+  <si>
+    <t>DepartureArrivalTimeHelper.deltaj</t>
+  </si>
+  <si>
+    <t>--- no directly mapped feature. Code reuse delta ---</t>
+  </si>
+  <si>
+    <t>2017-09-22T00:00</t>
+  </si>
+  <si>
+    <t>ttsNavi.deltaj</t>
+  </si>
+  <si>
+    <t>tts.deltaj</t>
+  </si>
+  <si>
+    <t>--- no directly mapped feature. Code reuse &amp; feature interaction ---</t>
+  </si>
+  <si>
+    <t>--- no directly mapped delta. Just used in feature interaction. ----</t>
+  </si>
+  <si>
+    <t>SuggestionsHistory.deltaj</t>
+  </si>
+  <si>
+    <t>SuggestionsFavorites.deltaj</t>
+  </si>
+  <si>
+    <t>ArrivalTime.deltaj</t>
+  </si>
+  <si>
+    <t>DepartureTime.deltaj</t>
+  </si>
+  <si>
+    <t>0ee9151e0cb9820592d18e1df7b612b966f58d9b</t>
+  </si>
+  <si>
+    <t>0ee9151e0cb9820592d18e1df7b612b966f58d9b , 768fca3dca7fb0f2c3f2af2d90af00804b664c9a</t>
+  </si>
+  <si>
+    <t>27a855812a7651ff23980341b8c215a383ef1fa1</t>
+  </si>
+  <si>
+    <t>95f8baefc608fe1db620c141968cb30a9f282a38 , 2badc7e8952e341e4ad0566225c3bfe7bec3d2c7</t>
+  </si>
+  <si>
+    <t>38ffe2e73b3b967311ccbeb408b91b1950ee586a , 4b5b87fab1166b690c9859b54ace76e8337bc700 , 82ecc5181e4d99d15042527271a021ed07d69963</t>
+  </si>
+  <si>
+    <t>Kilometer</t>
+  </si>
+  <si>
+    <t>Mile</t>
+  </si>
+  <si>
+    <t>RouteDistanceMile.deltaj</t>
+  </si>
+  <si>
+    <t>--- does not have a mapped delta. Functionality realized in RouteDistanceMile.deltaj which is a feature interaction delta ---</t>
+  </si>
+  <si>
+    <t>2017-09-25T00:00</t>
   </si>
 </sst>
 </file>
@@ -953,16 +1061,19 @@
   <threadedComment ref="O1" dT="2021-06-23T12:59:04.88" personId="{D79E35A8-37B6-4A3D-A377-51485C625214}" id="{EC9143AF-697E-4544-ABFB-F004AC1C52AD}">
     <text>not considered the last commit for migration to the new DeltaJ version</text>
   </threadedComment>
-  <threadedComment ref="D34" dT="2021-06-25T12:05:07.49" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{02B7A502-EA60-48C2-A4ED-6D65727931AC}">
+  <threadedComment ref="D33" dT="2021-06-25T12:05:07.49" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{02B7A502-EA60-48C2-A4ED-6D65727931AC}">
     <text>before the feature was introduced</text>
   </threadedComment>
-  <threadedComment ref="D37" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{6207ED8D-94FE-4AAF-8444-4D21B004E5BF}">
+  <threadedComment ref="D36" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{6207ED8D-94FE-4AAF-8444-4D21B004E5BF}">
     <text>before feature was introduced</text>
   </threadedComment>
-  <threadedComment ref="D38" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{083D291C-1366-47CF-A1C9-0188B7497467}">
+  <threadedComment ref="D37" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{083D291C-1366-47CF-A1C9-0188B7497467}">
     <text>before feature was introduced</text>
   </threadedComment>
-  <threadedComment ref="D39" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{0850F9F9-4BB2-4AA3-B45A-D7482D0EB600}">
+  <threadedComment ref="D38" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{0850F9F9-4BB2-4AA3-B45A-D7482D0EB600}">
+    <text>before feature was introduced</text>
+  </threadedComment>
+  <threadedComment ref="D40" dT="2021-06-25T12:13:24.65" personId="{363638F8-A791-4E0F-8248-B1C5ADE4E115}" id="{E1EEB336-76F9-4E42-854F-F43347D1E75F}">
     <text>before feature was introduced</text>
   </threadedComment>
 </ThreadedComments>
@@ -970,11 +1081,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q50"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1015,7 +1126,7 @@
         <v>13</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>31</v>
@@ -1048,7 +1159,7 @@
         <v>25</v>
       </c>
       <c r="Q1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -1059,7 +1170,7 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1068,7 +1179,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" s="4">
         <v>7</v>
@@ -1080,13 +1191,13 @@
         <v>4</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="M2" s="2">
         <v>4</v>
@@ -1112,7 +1223,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1121,7 +1232,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G3" s="4">
         <v>3</v>
@@ -1133,13 +1244,13 @@
         <v>3</v>
       </c>
       <c r="J3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="K3" s="3">
-        <v>1</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="M3" s="2">
         <v>2</v>
@@ -1165,7 +1276,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>23</v>
@@ -1174,7 +1285,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="4">
         <v>1</v>
@@ -1189,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M4" s="2">
         <v>2</v>
@@ -1209,19 +1320,19 @@
     </row>
     <row r="5" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="G5" s="4">
         <v>2</v>
@@ -1234,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M5" s="2">
         <v>1</v>
@@ -1260,7 +1371,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -1269,7 +1380,7 @@
         <v>28</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="4">
         <v>8</v>
@@ -1281,13 +1392,13 @@
         <v>8</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K6" s="2">
         <v>7</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M6" s="2">
         <v>4</v>
@@ -1305,9 +1416,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>35</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -1319,7 +1430,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -1331,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -1346,15 +1457,15 @@
         <v>27</v>
       </c>
       <c r="Q7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
         <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1366,7 +1477,7 @@
         <v>28</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -1381,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -1401,22 +1512,22 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -1431,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -1451,10 +1562,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1466,7 +1577,7 @@
         <v>19</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="3">
         <v>3</v>
@@ -1478,13 +1589,13 @@
         <v>3</v>
       </c>
       <c r="J10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="K10" s="3">
-        <v>2</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="M10" s="3">
         <v>1</v>
@@ -1504,19 +1615,19 @@
     </row>
     <row r="11" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="G11" s="3">
         <v>2</v>
@@ -1525,7 +1636,7 @@
         <v>5</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K11">
         <v>2</v>
@@ -1534,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O11">
         <v>2</v>
@@ -1548,13 +1659,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
@@ -1563,7 +1674,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G12" s="3">
         <v>3</v>
@@ -1578,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -1598,10 +1709,10 @@
     </row>
     <row r="13" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
@@ -1610,7 +1721,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="3">
         <v>1</v>
@@ -1619,19 +1730,19 @@
         <v>1</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O13">
         <v>2</v>
@@ -1643,98 +1754,104 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>70</v>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="3">
         <v>12</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1</v>
-      </c>
       <c r="H14" s="3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="I14" s="3">
+        <v>8</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="K14" s="3">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="O14">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="P14" t="s">
         <v>26</v>
       </c>
       <c r="Q14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" t="s">
-        <v>79</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" t="s">
-        <v>80</v>
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="G15" s="3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H15" s="3">
+        <v>9</v>
+      </c>
+      <c r="I15" s="3">
+        <v>13</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15">
         <v>7</v>
       </c>
-      <c r="I15" s="3">
-        <v>8</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" s="3">
-        <v>3</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M15" s="3">
-        <v>1</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O15">
-        <v>16</v>
-      </c>
       <c r="P15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q15" t="s">
         <v>26</v>
@@ -1742,49 +1859,49 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>68</v>
+      <c r="E16" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G16" s="3">
+        <v>4</v>
+      </c>
+      <c r="H16" s="3">
+        <v>4</v>
+      </c>
+      <c r="I16" s="3">
+        <v>8</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M16" s="3">
+        <v>2</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16">
         <v>6</v>
       </c>
-      <c r="H16" s="3">
-        <v>9</v>
-      </c>
-      <c r="I16" s="3">
-        <v>13</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="M16" s="3">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O16">
-        <v>7</v>
-      </c>
       <c r="P16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q16" t="s">
         <v>26</v>
@@ -1792,28 +1909,28 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>65</v>
+        <v>96</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="G17" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H17" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I17" s="3">
         <v>8</v>
@@ -1821,17 +1938,14 @@
       <c r="K17" s="3">
         <v>0</v>
       </c>
-      <c r="L17" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="M17" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="O17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="P17" t="s">
         <v>26</v>
@@ -1848,25 +1962,25 @@
         <v>93</v>
       </c>
       <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>98</v>
       </c>
       <c r="G18" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K18" s="3">
         <v>0</v>
@@ -1875,10 +1989,10 @@
         <v>0</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="O18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P18" t="s">
         <v>26</v>
@@ -1895,25 +2009,25 @@
         <v>94</v>
       </c>
       <c r="C19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>99</v>
-      </c>
       <c r="G19" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K19" s="3">
         <v>0</v>
@@ -1922,10 +2036,10 @@
         <v>0</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="O19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P19" t="s">
         <v>26</v>
@@ -1936,281 +2050,284 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>3</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" s="3">
+        <v>2</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O20">
+        <v>5</v>
+      </c>
+      <c r="P20" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K21" s="3">
+        <v>3</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M21" s="3">
+        <v>1</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="P21" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="3">
-        <v>1</v>
-      </c>
-      <c r="H20" s="3">
-        <v>1</v>
-      </c>
-      <c r="I20" s="3">
+      <c r="E22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
         <v>8</v>
       </c>
-      <c r="K20" s="3">
-        <v>0</v>
-      </c>
-      <c r="M20" s="3">
-        <v>0</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K23" s="3">
+        <v>2</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O23">
+        <v>2</v>
+      </c>
+      <c r="P23" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G21" s="3">
-        <v>2</v>
-      </c>
-      <c r="H21" s="3">
-        <v>1</v>
-      </c>
-      <c r="I21" s="3">
-        <v>3</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="K21" s="3">
-        <v>2</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M21" s="3">
-        <v>1</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O21">
-        <v>5</v>
-      </c>
-      <c r="P21" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="3">
-        <v>3</v>
-      </c>
-      <c r="H22" s="3">
-        <v>2</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22" s="3">
-        <v>3</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M22" s="3">
-        <v>1</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O22">
-        <v>4</v>
-      </c>
-      <c r="P22" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="D24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" s="3">
-        <v>1</v>
-      </c>
-      <c r="H23" s="3">
-        <v>1</v>
-      </c>
-      <c r="I23" s="3">
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
+        <v>1</v>
+      </c>
+      <c r="I24" s="3">
         <v>8</v>
       </c>
-      <c r="K23" s="3">
-        <v>0</v>
-      </c>
-      <c r="M23" s="3">
-        <v>0</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G24" s="3">
-        <v>1</v>
-      </c>
-      <c r="H24" s="3">
-        <v>1</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>110</v>
-      </c>
       <c r="K24" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M24" s="3">
         <v>0</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="O24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P24" t="s">
         <v>26</v>
       </c>
       <c r="Q24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="G25" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I25" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K25" s="3">
         <v>0</v>
       </c>
+      <c r="L25" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="M25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="O25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P25" t="s">
         <v>26</v>
@@ -2219,162 +2336,161 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>2</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="K26" s="3">
+        <v>2</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3">
+        <v>9</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
         <v>113</v>
       </c>
-      <c r="B26" t="s">
-        <v>118</v>
-      </c>
-      <c r="C26" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="G26" s="3">
-        <v>3</v>
-      </c>
-      <c r="H26" s="3">
-        <v>2</v>
-      </c>
-      <c r="I26" s="3">
-        <v>9</v>
-      </c>
-      <c r="K26" s="3">
-        <v>0</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="M26" s="3">
-        <v>1</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O26">
-        <v>4</v>
-      </c>
-      <c r="P26" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="G27" s="3">
-        <v>2</v>
-      </c>
-      <c r="H27" s="3">
-        <v>2</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="K27" s="3">
-        <v>2</v>
-      </c>
-      <c r="M27" s="3">
-        <v>0</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O27">
-        <v>2</v>
-      </c>
-      <c r="P27" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q27" t="s">
+      <c r="D28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" t="s">
+        <v>115</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+      <c r="I28"/>
+      <c r="J28" t="s">
+        <v>115</v>
+      </c>
+      <c r="K28" s="3">
+        <v>2</v>
+      </c>
+      <c r="L28"/>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O28">
+        <v>2</v>
+      </c>
+      <c r="P28" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C28" t="s">
-        <v>101</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="G28" s="3">
-        <v>1</v>
-      </c>
-      <c r="H28" s="3">
-        <v>1</v>
-      </c>
-      <c r="I28" s="3">
-        <v>9</v>
-      </c>
-      <c r="K28" s="3">
-        <v>0</v>
-      </c>
-      <c r="M28" s="3">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O28">
-        <v>1</v>
-      </c>
-      <c r="P28" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>124</v>
+      </c>
+      <c r="C29" t="s">
+        <v>100</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" t="s">
-        <v>116</v>
+        <v>28</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="G29" s="3">
         <v>1</v>
@@ -2382,39 +2498,37 @@
       <c r="H29" s="3">
         <v>1</v>
       </c>
-      <c r="I29"/>
-      <c r="J29" t="s">
-        <v>116</v>
+      <c r="I29" s="3">
+        <v>1</v>
       </c>
       <c r="K29" s="3">
-        <v>2</v>
-      </c>
-      <c r="L29"/>
+        <v>0</v>
+      </c>
       <c r="M29" s="3">
         <v>0</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="O29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P29" t="s">
         <v>26</v>
       </c>
       <c r="Q29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>28</v>
@@ -2423,7 +2537,7 @@
         <v>28</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G30" s="3">
         <v>1</v>
@@ -2461,7 +2575,7 @@
         <v>129</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>28</v>
@@ -2470,7 +2584,7 @@
         <v>28</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G31" s="3">
         <v>1</v>
@@ -2502,22 +2616,22 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="G32" s="3">
         <v>1</v>
@@ -2531,14 +2645,17 @@
       <c r="K32" s="3">
         <v>0</v>
       </c>
+      <c r="L32" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="M32" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="O32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P32" t="s">
         <v>26</v>
@@ -2549,22 +2666,22 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B33" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="G33" s="3">
         <v>1</v>
@@ -2573,22 +2690,22 @@
         <v>1</v>
       </c>
       <c r="I33" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" s="3">
         <v>0</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="M33" s="3">
         <v>2</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="O33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P33" t="s">
         <v>26</v>
@@ -2605,16 +2722,16 @@
         <v>145</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>28</v>
+        <v>137</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G34" s="3">
         <v>1</v>
@@ -2623,22 +2740,19 @@
         <v>1</v>
       </c>
       <c r="I34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="3">
         <v>0</v>
       </c>
-      <c r="L34" s="8" t="s">
-        <v>152</v>
-      </c>
       <c r="M34" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="O34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P34" t="s">
         <v>26</v>
@@ -2651,58 +2765,58 @@
       <c r="A35" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="13" t="s">
         <v>146</v>
       </c>
       <c r="C35" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G35" s="3">
-        <v>1</v>
-      </c>
-      <c r="H35" s="3">
-        <v>1</v>
-      </c>
-      <c r="I35" s="3">
-        <v>1</v>
-      </c>
-      <c r="K35" s="3">
-        <v>0</v>
-      </c>
-      <c r="M35" s="3">
-        <v>0</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="O35">
-        <v>1</v>
-      </c>
-      <c r="P35" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" t="s">
         <v>147</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" s="3">
+        <v>8</v>
+      </c>
+      <c r="H36" s="3">
+        <v>7</v>
+      </c>
+      <c r="I36" s="3">
+        <v>3</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0</v>
+      </c>
+      <c r="M36" s="3">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O36">
+        <v>8</v>
+      </c>
+      <c r="P36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -2713,37 +2827,40 @@
         <v>148</v>
       </c>
       <c r="C37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>154</v>
       </c>
       <c r="G37" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H37" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I37" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K37" s="3">
         <v>0</v>
       </c>
+      <c r="L37" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="M37" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="O37">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P37" t="s">
         <v>26</v>
@@ -2760,7 +2877,7 @@
         <v>149</v>
       </c>
       <c r="C38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>28</v>
@@ -2772,19 +2889,19 @@
         <v>155</v>
       </c>
       <c r="G38" s="3">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3">
+        <v>4</v>
+      </c>
+      <c r="I38" s="3">
         <v>3</v>
       </c>
-      <c r="H38" s="3">
-        <v>5</v>
-      </c>
-      <c r="I38" s="3">
-        <v>4</v>
-      </c>
       <c r="K38" s="3">
         <v>0</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M38" s="3">
         <v>1</v>
@@ -2793,7 +2910,7 @@
         <v>12</v>
       </c>
       <c r="O38">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P38" t="s">
         <v>26</v>
@@ -2804,56 +2921,474 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B39" t="s">
-        <v>150</v>
+        <v>156</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>138</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="G39" s="3">
-        <v>1</v>
-      </c>
-      <c r="H39" s="3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="M40" s="3">
+        <v>1</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O40">
+        <v>2</v>
+      </c>
+      <c r="P40" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B41" t="s">
+        <v>178</v>
+      </c>
+      <c r="C41" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="G41" s="3">
+        <v>1</v>
+      </c>
+      <c r="H41" s="3">
+        <v>1</v>
+      </c>
+      <c r="I41" s="3">
+        <v>5</v>
+      </c>
+      <c r="K41" s="3">
+        <v>0</v>
+      </c>
+      <c r="M41" s="3">
+        <v>0</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B42" t="s">
+        <v>179</v>
+      </c>
+      <c r="C42" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="G42" s="3">
+        <v>1</v>
+      </c>
+      <c r="H42" s="3">
+        <v>1</v>
+      </c>
+      <c r="I42" s="3">
+        <v>5</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="M42" s="3">
+        <v>0</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G43" s="3">
+        <v>2</v>
+      </c>
+      <c r="H43" s="3">
+        <v>1</v>
+      </c>
+      <c r="I43" s="3">
+        <v>5</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O43">
+        <v>2</v>
+      </c>
+      <c r="P43" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" s="3">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3">
+        <v>1</v>
+      </c>
+      <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="I39" s="3">
+      <c r="K44" s="3">
+        <v>0</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G45" s="3">
+        <v>1</v>
+      </c>
+      <c r="H45" s="3">
+        <v>1</v>
+      </c>
+      <c r="I45" s="3">
+        <v>4</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0</v>
+      </c>
+      <c r="M45" s="3">
+        <v>0</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" t="s">
+        <v>173</v>
+      </c>
+      <c r="C47" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G47" s="3">
+        <v>2</v>
+      </c>
+      <c r="H47" s="3">
+        <v>2</v>
+      </c>
+      <c r="I47" s="3">
+        <v>5</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0</v>
+      </c>
+      <c r="M47" s="3">
+        <v>0</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O47">
+        <v>2</v>
+      </c>
+      <c r="P47" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" t="s">
+        <v>172</v>
+      </c>
+      <c r="C48" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="G48" s="3">
         <v>3</v>
       </c>
-      <c r="K39" s="3">
-        <v>0</v>
-      </c>
-      <c r="L39" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M39" s="3">
-        <v>1</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O39">
-        <v>2</v>
-      </c>
-      <c r="P39" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="H48" s="3">
+        <v>2</v>
+      </c>
+      <c r="I48" s="3">
+        <v>5</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0</v>
+      </c>
+      <c r="M48" s="3">
+        <v>0</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O48">
+        <v>3</v>
+      </c>
+      <c r="P48" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" t="s">
+        <v>189</v>
+      </c>
+      <c r="N50" s="1"/>
+    </row>
+    <row r="51" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" t="s">
+        <v>187</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G51" s="3">
+        <v>1</v>
+      </c>
+      <c r="H51" s="3">
+        <v>1</v>
+      </c>
+      <c r="I51" s="3">
+        <v>1</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0</v>
+      </c>
+      <c r="M51" s="3">
+        <v>0</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="P51" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A52"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A53" s="5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>